<commit_message>
server backup + api search keyword update
</commit_message>
<xml_diff>
--- a/templates/NotBuyCustomers.xlsx
+++ b/templates/NotBuyCustomers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Last 6 months" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,7 +64,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -109,12 +109,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -186,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,10 +214,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,15 +312,16 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="59.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
@@ -360,7 +351,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -374,20 +365,20 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -414,13 +405,14 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="59.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="32.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -448,7 +440,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -462,20 +454,20 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -498,17 +490,18 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="59.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -536,7 +529,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -550,20 +543,20 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -586,15 +579,16 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="59.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="32.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
@@ -624,7 +618,7 @@
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -638,20 +632,20 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>